<commit_message>
sn from new process
</commit_message>
<xml_diff>
--- a/data/sen/sn_match_ego_alter_organizations_2025-09-23_KEY.xlsx
+++ b/data/sen/sn_match_ego_alter_organizations_2025-09-23_KEY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucdavis365-my.sharepoint.com/personal/marfisher_ucdavis_edu/Documents/Documents/russian/data/sen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:40009_{DA35E2E0-F40F-47BB-B568-810BF0932543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B5FCA63-D7AA-4598-AA53-DB0D97314AB2}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:40009_{DA35E2E0-F40F-47BB-B568-810BF0932543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0844BFF-9237-4494-A44D-E4EAE40E63A4}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="304">
   <si>
     <t>org_name</t>
   </si>
@@ -947,6 +947,9 @@
   </si>
   <si>
     <t>NOAA Cordell Bank National Marine Sanctuary - Advisory Council</t>
+  </si>
+  <si>
+    <t>Photographer 1</t>
   </si>
 </sst>
 </file>
@@ -6806,10 +6809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D216"/>
+  <dimension ref="A1:D226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="A230" sqref="A230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9844,6 +9847,146 @@
         <v>231</v>
       </c>
     </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>265</v>
+      </c>
+      <c r="B217" t="s">
+        <v>265</v>
+      </c>
+      <c r="C217" t="s">
+        <v>85</v>
+      </c>
+      <c r="D217" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>268</v>
+      </c>
+      <c r="B218" t="s">
+        <v>268</v>
+      </c>
+      <c r="C218" t="s">
+        <v>85</v>
+      </c>
+      <c r="D218" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>272</v>
+      </c>
+      <c r="B219" t="s">
+        <v>272</v>
+      </c>
+      <c r="C219" t="s">
+        <v>85</v>
+      </c>
+      <c r="D219" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>266</v>
+      </c>
+      <c r="B220" t="s">
+        <v>266</v>
+      </c>
+      <c r="C220" t="s">
+        <v>85</v>
+      </c>
+      <c r="D220" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>269</v>
+      </c>
+      <c r="B221" t="s">
+        <v>269</v>
+      </c>
+      <c r="C221" t="s">
+        <v>85</v>
+      </c>
+      <c r="D221" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>270</v>
+      </c>
+      <c r="B222" t="s">
+        <v>270</v>
+      </c>
+      <c r="C222" t="s">
+        <v>85</v>
+      </c>
+      <c r="D222" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>271</v>
+      </c>
+      <c r="B223" t="s">
+        <v>271</v>
+      </c>
+      <c r="C223" t="s">
+        <v>85</v>
+      </c>
+      <c r="D223" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>267</v>
+      </c>
+      <c r="B224" t="s">
+        <v>267</v>
+      </c>
+      <c r="C224" t="s">
+        <v>85</v>
+      </c>
+      <c r="D224" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>303</v>
+      </c>
+      <c r="B225" t="s">
+        <v>295</v>
+      </c>
+      <c r="C225" t="s">
+        <v>85</v>
+      </c>
+      <c r="D225" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>273</v>
+      </c>
+      <c r="B226" t="s">
+        <v>273</v>
+      </c>
+      <c r="C226" t="s">
+        <v>85</v>
+      </c>
+      <c r="D226" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D216" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D216">

</xml_diff>